<commit_message>
Actualización del archivo principal
</commit_message>
<xml_diff>
--- a/Muestra de farmacias.xlsx
+++ b/Muestra de farmacias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo i5\Documents\MAESTRIA IA YACHAY TECH\FUNDAMETOS DE INTELIGENCIA ARTIFICIAL\SEMANA 4\Examen Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19173EF0-DF34-441C-9712-1D7CC71B890B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79374E4-1DD6-45B2-BDE5-CA315793443A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12006,7 +12006,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12016,6 +12016,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -12069,7 +12077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -12085,6 +12093,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -62317,7 +62328,7 @@
   <dimension ref="A1:J991"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62444,7 +62455,7 @@
       <c r="E4">
         <v>9600</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>5</v>
       </c>
       <c r="G4" t="s">
@@ -94047,5 +94058,6 @@
   </sheetData>
   <autoFilter ref="A1:F991" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>